<commit_message>
Updated tracker, updated to generate needed columns next to each other in CSV
</commit_message>
<xml_diff>
--- a/ElectionTracker2020.xlsx
+++ b/ElectionTracker2020.xlsx
@@ -236,14 +236,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="7">
+  <numFmts count="6">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="#,##0"/>
     <numFmt numFmtId="166" formatCode="0.00%"/>
     <numFmt numFmtId="167" formatCode="0.0%"/>
-    <numFmt numFmtId="168" formatCode="0%"/>
-    <numFmt numFmtId="169" formatCode="#,##0.00000"/>
-    <numFmt numFmtId="170" formatCode="#,##0.000000"/>
+    <numFmt numFmtId="168" formatCode="#,##0.00000"/>
+    <numFmt numFmtId="169" formatCode="#,##0.000000"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -319,7 +318,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -344,7 +343,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -352,15 +351,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -407,11 +402,11 @@
   <dimension ref="A1:Q52"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B26" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B17" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A26" activeCellId="0" sqref="A26"/>
-      <selection pane="bottomRight" activeCell="G33" activeCellId="0" sqref="G33"/>
+      <selection pane="bottomLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
+      <selection pane="bottomRight" activeCell="G1" activeCellId="0" sqref="G:G G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -443,13 +438,13 @@
       <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="6" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="5" t="s">
@@ -617,41 +612,41 @@
         <v>0.9</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>0.485293103622942</v>
+        <v>0.485833713549296</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>0.500669438537634</v>
+        <v>0.499850955342635</v>
       </c>
       <c r="F4" s="2" t="n">
         <f aca="false">1-(D4+E4)</f>
-        <v>0.0140374578394243</v>
+        <v>0.0143153311080694</v>
       </c>
       <c r="G4" s="0" t="n">
-        <v>3060027</v>
+        <v>3123225</v>
       </c>
       <c r="H4" s="1" t="n">
         <f aca="false">(G4/C4)-G4</f>
-        <v>340003</v>
+        <v>347025</v>
       </c>
       <c r="I4" s="1" t="n">
         <f aca="false">G4+H4</f>
-        <v>3400030</v>
+        <v>3470250</v>
       </c>
       <c r="J4" s="1" t="n">
         <f aca="false">G4*D4</f>
-        <v>1485010</v>
+        <v>1517368</v>
       </c>
       <c r="K4" s="1" t="n">
         <f aca="false">G4*E4</f>
-        <v>1532062</v>
+        <v>1561147</v>
       </c>
       <c r="L4" s="3" t="n">
         <f aca="false">((G4*(D4/100))/I4)*100</f>
-        <v>0.436763793260648</v>
+        <v>0.437250342194367</v>
       </c>
       <c r="M4" s="3" t="n">
         <f aca="false">((G4*(E4/100))/I4)*100</f>
-        <v>0.45060249468387</v>
+        <v>0.449865859808371</v>
       </c>
       <c r="N4" s="3" t="n">
         <f aca="false">H4/I4</f>
@@ -676,60 +671,60 @@
         <v>6</v>
       </c>
       <c r="C5" s="2" t="n">
-        <v>0.93</v>
+        <v>0.99</v>
       </c>
       <c r="D5" s="2" t="n">
-        <v>0.636893986130917</v>
+        <v>0.636877491571526</v>
       </c>
       <c r="E5" s="2" t="n">
-        <v>0.352119299736036</v>
+        <v>0.352135367907842</v>
       </c>
       <c r="F5" s="2" t="n">
         <f aca="false">1-(D5+E5)</f>
-        <v>0.0109867141330475</v>
+        <v>0.0109871405206314</v>
       </c>
       <c r="G5" s="0" t="n">
-        <v>1186524</v>
+        <v>1186751</v>
       </c>
       <c r="H5" s="1" t="n">
         <f aca="false">(G5/C5)-G5</f>
-        <v>89308.2580645161</v>
+        <v>11987.3838383839</v>
       </c>
       <c r="I5" s="1" t="n">
         <f aca="false">G5+H5</f>
-        <v>1275832.25806452</v>
+        <v>1198738.38383838</v>
       </c>
       <c r="J5" s="1" t="n">
         <f aca="false">G5*D5</f>
-        <v>755690</v>
+        <v>755815</v>
       </c>
       <c r="K5" s="1" t="n">
         <f aca="false">G5*E5</f>
-        <v>417798</v>
+        <v>417897</v>
       </c>
       <c r="L5" s="3" t="n">
         <f aca="false">((G5*(D5/100))/I5)*100</f>
-        <v>0.592311407101753</v>
+        <v>0.630508716655811</v>
       </c>
       <c r="M5" s="3" t="n">
         <f aca="false">((G5*(E5/100))/I5)*100</f>
-        <v>0.327470948754513</v>
+        <v>0.348614014228764</v>
       </c>
       <c r="N5" s="3" t="n">
         <f aca="false">H5/I5</f>
-        <v>0.07</v>
+        <v>0.0100000000000001</v>
       </c>
       <c r="O5" s="0" t="str">
         <f aca="false">IF(SUM(MIN(L5,M5),N5)&lt;MAX(L5,M5),IF(MAX(L5,M5)=L5,"Trump","Biden"),"NONE")</f>
         <v>Trump</v>
       </c>
-      <c r="P5" s="9" t="n">
+      <c r="P5" s="8" t="n">
         <f aca="false">SUM(J2:J52)/SUM(G2:G52)</f>
-        <v>0.481279031132727</v>
+        <v>0.481045766883744</v>
       </c>
       <c r="Q5" s="0" t="n">
         <f aca="false">SUM(K2:K52)/SUM(G2:G52)</f>
-        <v>0.507066151932812</v>
+        <v>0.507295222284099</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -796,54 +791,54 @@
         <v>9</v>
       </c>
       <c r="C7" s="2" t="n">
-        <v>0.92</v>
+        <v>0.93</v>
       </c>
       <c r="D7" s="2" t="n">
-        <v>0.426122374176101</v>
+        <v>0.426430236398206</v>
       </c>
       <c r="E7" s="2" t="n">
-        <v>0.55804788554717</v>
+        <v>0.557565351775792</v>
       </c>
       <c r="F7" s="2" t="n">
         <f aca="false">1-(D7+E7)</f>
-        <v>0.0158297402767289</v>
+        <v>0.0160044118260022</v>
       </c>
       <c r="G7" s="0" t="n">
-        <v>3088364</v>
+        <v>3118890</v>
       </c>
       <c r="H7" s="1" t="n">
         <f aca="false">(G7/C7)-G7</f>
-        <v>268553.391304348</v>
+        <v>234755.161290322</v>
       </c>
       <c r="I7" s="1" t="n">
         <f aca="false">G7+H7</f>
-        <v>3356917.39130435</v>
+        <v>3353645.16129032</v>
       </c>
       <c r="J7" s="1" t="n">
         <f aca="false">G7*D7</f>
-        <v>1316021</v>
+        <v>1329989</v>
       </c>
       <c r="K7" s="1" t="n">
         <f aca="false">G7*E7</f>
-        <v>1723455</v>
+        <v>1738985</v>
       </c>
       <c r="L7" s="3" t="n">
         <f aca="false">((G7*(D7/100))/I7)*100</f>
-        <v>0.392032584242013</v>
+        <v>0.396580119850331</v>
       </c>
       <c r="M7" s="3" t="n">
         <f aca="false">((G7*(E7/100))/I7)*100</f>
-        <v>0.513404054703396</v>
+        <v>0.518535777151487</v>
       </c>
       <c r="N7" s="3" t="n">
         <f aca="false">H7/I7</f>
-        <v>0.08</v>
+        <v>0.07</v>
       </c>
       <c r="O7" s="0" t="str">
         <f aca="false">IF(SUM(MIN(L7,M7),N7)&lt;MAX(L7,M7),IF(MAX(L7,M7)=L7,"Trump","Biden"),"NONE")</f>
         <v>Biden</v>
       </c>
-      <c r="P7" s="10"/>
+      <c r="P7" s="9"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
@@ -856,45 +851,45 @@
         <v>0.99</v>
       </c>
       <c r="D8" s="2" t="n">
-        <v>0.406079302973037</v>
+        <v>0.405644476153639</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>0.582730424275798</v>
+        <v>0.583157426700528</v>
       </c>
       <c r="F8" s="2" t="n">
         <f aca="false">1-(D8+E8)</f>
-        <v>0.0111902727511655</v>
+        <v>0.0111980971458321</v>
       </c>
       <c r="G8" s="0" t="n">
-        <v>1757866</v>
+        <v>1763246</v>
       </c>
       <c r="H8" s="1" t="n">
         <f aca="false">(G8/C8)-G8</f>
-        <v>17756.2222222223</v>
+        <v>17810.5656565656</v>
       </c>
       <c r="I8" s="1" t="n">
         <f aca="false">G8+H8</f>
-        <v>1775622.22222222</v>
+        <v>1781056.56565657</v>
       </c>
       <c r="J8" s="1" t="n">
         <f aca="false">G8*D8</f>
-        <v>713833</v>
+        <v>715251</v>
       </c>
       <c r="K8" s="1" t="n">
         <f aca="false">G8*E8</f>
-        <v>1024362</v>
+        <v>1028250</v>
       </c>
       <c r="L8" s="3" t="n">
         <f aca="false">((G8*(D8/100))/I8)*100</f>
-        <v>0.402018509943306</v>
+        <v>0.401588031392103</v>
       </c>
       <c r="M8" s="3" t="n">
         <f aca="false">((G8*(E8/100))/I8)*100</f>
-        <v>0.57690312003304</v>
+        <v>0.577325852433523</v>
       </c>
       <c r="N8" s="3" t="n">
         <f aca="false">H8/I8</f>
-        <v>0.01</v>
+        <v>0.00999999999999996</v>
       </c>
       <c r="O8" s="0" t="str">
         <f aca="false">IF(SUM(MIN(L8,M8),N8)&lt;MAX(L8,M8),IF(MAX(L8,M8)=L8,"Trump","Biden"),"NONE")</f>
@@ -1080,45 +1075,45 @@
         <v>0.99</v>
       </c>
       <c r="D12" s="2" t="n">
-        <v>0.493719053759625</v>
+        <v>0.493654719486346</v>
       </c>
       <c r="E12" s="2" t="n">
-        <v>0.493903962429462</v>
+        <v>0.493968616727235</v>
       </c>
       <c r="F12" s="2" t="n">
         <f aca="false">1-(D12+E12)</f>
-        <v>0.0123769838109131</v>
+        <v>0.0123766637864192</v>
       </c>
       <c r="G12" s="0" t="n">
-        <v>4959205</v>
+        <v>4960222</v>
       </c>
       <c r="H12" s="1" t="n">
         <f aca="false">(G12/C12)-G12</f>
-        <v>50092.9797979798</v>
+        <v>50103.2525252523</v>
       </c>
       <c r="I12" s="1" t="n">
         <f aca="false">G12+H12</f>
-        <v>5009297.97979798</v>
+        <v>5010325.25252525</v>
       </c>
       <c r="J12" s="1" t="n">
         <f aca="false">G12*D12</f>
-        <v>2448454</v>
+        <v>2448637</v>
       </c>
       <c r="K12" s="1" t="n">
         <f aca="false">G12*E12</f>
-        <v>2449371</v>
+        <v>2450194</v>
       </c>
       <c r="L12" s="3" t="n">
         <f aca="false">((G12*(D12/100))/I12)*100</f>
-        <v>0.488781863222029</v>
+        <v>0.488718172291482</v>
       </c>
       <c r="M12" s="3" t="n">
         <f aca="false">((G12*(E12/100))/I12)*100</f>
-        <v>0.488964922805167</v>
+        <v>0.489028930559963</v>
       </c>
       <c r="N12" s="3" t="n">
         <f aca="false">H12/I12</f>
-        <v>0.01</v>
+        <v>0.00999999999999995</v>
       </c>
       <c r="O12" s="0" t="str">
         <f aca="false">IF(SUM(MIN(L12,M12),N12)&lt;MAX(L12,M12),IF(MAX(L12,M12)=L12,"Trump","Biden"),"NONE")</f>
@@ -1248,41 +1243,41 @@
         <v>0.91</v>
       </c>
       <c r="D15" s="2" t="n">
-        <v>0.429048599868547</v>
+        <v>0.428698584803474</v>
       </c>
       <c r="E15" s="2" t="n">
-        <v>0.559892053925889</v>
+        <v>0.560249450513916</v>
       </c>
       <c r="F15" s="2" t="n">
         <f aca="false">1-(D15+E15)</f>
-        <v>0.0110593462055634</v>
+        <v>0.0110519646826102</v>
       </c>
       <c r="G15" s="0" t="n">
-        <v>5344891</v>
+        <v>5349999</v>
       </c>
       <c r="H15" s="1" t="n">
         <f aca="false">(G15/C15)-G15</f>
-        <v>528615.593406593</v>
+        <v>529120.78021978</v>
       </c>
       <c r="I15" s="1" t="n">
         <f aca="false">G15+H15</f>
-        <v>5873506.59340659</v>
+        <v>5879119.78021978</v>
       </c>
       <c r="J15" s="1" t="n">
         <f aca="false">G15*D15</f>
-        <v>2293218</v>
+        <v>2293537</v>
       </c>
       <c r="K15" s="1" t="n">
         <f aca="false">G15*E15</f>
-        <v>2992562</v>
+        <v>2997334</v>
       </c>
       <c r="L15" s="3" t="n">
         <f aca="false">((G15*(D15/100))/I15)*100</f>
-        <v>0.390434225880378</v>
+        <v>0.390115712171161</v>
       </c>
       <c r="M15" s="3" t="n">
         <f aca="false">((G15*(E15/100))/I15)*100</f>
-        <v>0.509501769072559</v>
+        <v>0.509826999967664</v>
       </c>
       <c r="N15" s="3" t="n">
         <f aca="false">H15/I15</f>
@@ -1304,45 +1299,45 @@
         <v>0.99</v>
       </c>
       <c r="D16" s="2" t="n">
-        <v>0.572337188799026</v>
+        <v>0.570742854043356</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>0.40821150363162</v>
+        <v>0.409842409264938</v>
       </c>
       <c r="F16" s="2" t="n">
         <f aca="false">1-(D16+E16)</f>
-        <v>0.0194513075693545</v>
+        <v>0.0194147366917058</v>
       </c>
       <c r="G16" s="0" t="n">
-        <v>3008024</v>
+        <v>3023528</v>
       </c>
       <c r="H16" s="1" t="n">
         <f aca="false">(G16/C16)-G16</f>
-        <v>30384.0808080807</v>
+        <v>30540.6868686867</v>
       </c>
       <c r="I16" s="1" t="n">
         <f aca="false">G16+H16</f>
-        <v>3038408.08080808</v>
+        <v>3054068.68686869</v>
       </c>
       <c r="J16" s="1" t="n">
         <f aca="false">G16*D16</f>
-        <v>1721604</v>
+        <v>1725657</v>
       </c>
       <c r="K16" s="1" t="n">
         <f aca="false">G16*E16</f>
-        <v>1227910</v>
+        <v>1239170</v>
       </c>
       <c r="L16" s="3" t="n">
         <f aca="false">((G16*(D16/100))/I16)*100</f>
-        <v>0.566613816911035</v>
+        <v>0.565035425502923</v>
       </c>
       <c r="M16" s="3" t="n">
         <f aca="false">((G16*(E16/100))/I16)*100</f>
-        <v>0.404129388595304</v>
+        <v>0.405743985172289</v>
       </c>
       <c r="N16" s="3" t="n">
         <f aca="false">H16/I16</f>
-        <v>0.00999999999999998</v>
+        <v>0.00999999999999994</v>
       </c>
       <c r="O16" s="0" t="str">
         <f aca="false">IF(SUM(MIN(L16,M16),N16)&lt;MAX(L16,M16),IF(MAX(L16,M16)=L16,"Trump","Biden"),"NONE")</f>
@@ -1360,45 +1355,45 @@
         <v>0.99</v>
       </c>
       <c r="D17" s="2" t="n">
-        <v>0.535603903880216</v>
+        <v>0.535501522808662</v>
       </c>
       <c r="E17" s="2" t="n">
-        <v>0.452715768740752</v>
+        <v>0.452811458597295</v>
       </c>
       <c r="F17" s="2" t="n">
         <f aca="false">1-(D17+E17)</f>
-        <v>0.0116803273790316</v>
+        <v>0.0116870185940436</v>
       </c>
       <c r="G17" s="0" t="n">
-        <v>1673412</v>
+        <v>1673224</v>
       </c>
       <c r="H17" s="1" t="n">
         <f aca="false">(G17/C17)-G17</f>
-        <v>16903.1515151516</v>
+        <v>16901.2525252525</v>
       </c>
       <c r="I17" s="1" t="n">
         <f aca="false">G17+H17</f>
-        <v>1690315.15151515</v>
+        <v>1690125.25252525</v>
       </c>
       <c r="J17" s="1" t="n">
         <f aca="false">G17*D17</f>
-        <v>896286</v>
+        <v>896014</v>
       </c>
       <c r="K17" s="1" t="n">
         <f aca="false">G17*E17</f>
-        <v>757580</v>
+        <v>757655</v>
       </c>
       <c r="L17" s="3" t="n">
         <f aca="false">((G17*(D17/100))/I17)*100</f>
-        <v>0.530247864841414</v>
+        <v>0.530146507580575</v>
       </c>
       <c r="M17" s="3" t="n">
         <f aca="false">((G17*(E17/100))/I17)*100</f>
-        <v>0.448188611053345</v>
+        <v>0.448283344011322</v>
       </c>
       <c r="N17" s="3" t="n">
         <f aca="false">H17/I17</f>
-        <v>0.0100000000000001</v>
+        <v>0.01</v>
       </c>
       <c r="O17" s="0" t="str">
         <f aca="false">IF(SUM(MIN(L17,M17),N17)&lt;MAX(L17,M17),IF(MAX(L17,M17)=L17,"Trump","Biden"),"NONE")</f>
@@ -1416,45 +1411,45 @@
         <v>0.99</v>
       </c>
       <c r="D18" s="2" t="n">
-        <v>0.565309648921939</v>
+        <v>0.565310397345057</v>
       </c>
       <c r="E18" s="2" t="n">
-        <v>0.412637996697721</v>
+        <v>0.412630108983103</v>
       </c>
       <c r="F18" s="2" t="n">
         <f aca="false">1-(D18+E18)</f>
-        <v>0.0220523543803406</v>
+        <v>0.0220594936718395</v>
       </c>
       <c r="G18" s="0" t="n">
-        <v>1327568</v>
+        <v>1327637</v>
       </c>
       <c r="H18" s="1" t="n">
         <f aca="false">(G18/C18)-G18</f>
-        <v>13409.7777777778</v>
+        <v>13410.4747474748</v>
       </c>
       <c r="I18" s="1" t="n">
         <f aca="false">G18+H18</f>
-        <v>1340977.77777778</v>
+        <v>1341047.47474747</v>
       </c>
       <c r="J18" s="1" t="n">
         <f aca="false">G18*D18</f>
-        <v>750487</v>
+        <v>750527</v>
       </c>
       <c r="K18" s="1" t="n">
         <f aca="false">G18*E18</f>
-        <v>547805</v>
+        <v>547823</v>
       </c>
       <c r="L18" s="3" t="n">
         <f aca="false">((G18*(D18/100))/I18)*100</f>
-        <v>0.559656552432719</v>
+        <v>0.559657293371607</v>
       </c>
       <c r="M18" s="3" t="n">
         <f aca="false">((G18*(E18/100))/I18)*100</f>
-        <v>0.408511616730744</v>
+        <v>0.408503807893272</v>
       </c>
       <c r="N18" s="3" t="n">
         <f aca="false">H18/I18</f>
-        <v>0.00999999999999998</v>
+        <v>0.01</v>
       </c>
       <c r="O18" s="0" t="str">
         <f aca="false">IF(SUM(MIN(L18,M18),N18)&lt;MAX(L18,M18),IF(MAX(L18,M18)=L18,"Trump","Biden"),"NONE")</f>
@@ -1472,41 +1467,41 @@
         <v>0.98</v>
       </c>
       <c r="D19" s="2" t="n">
-        <v>0.628649379956062</v>
+        <v>0.627445838285178</v>
       </c>
       <c r="E19" s="2" t="n">
-        <v>0.358706015207552</v>
+        <v>0.36039320936152</v>
       </c>
       <c r="F19" s="2" t="n">
         <f aca="false">1-(D19+E19)</f>
-        <v>0.0126446048363857</v>
+        <v>0.0121609523533022</v>
       </c>
       <c r="G19" s="0" t="n">
-        <v>2092513</v>
+        <v>2101069</v>
       </c>
       <c r="H19" s="1" t="n">
         <f aca="false">(G19/C19)-G19</f>
-        <v>42704.3469387754</v>
+        <v>42878.9591836734</v>
       </c>
       <c r="I19" s="1" t="n">
         <f aca="false">G19+H19</f>
-        <v>2135217.34693878</v>
+        <v>2143947.95918367</v>
       </c>
       <c r="J19" s="1" t="n">
         <f aca="false">G19*D19</f>
-        <v>1315457</v>
+        <v>1318307</v>
       </c>
       <c r="K19" s="1" t="n">
         <f aca="false">G19*E19</f>
-        <v>750597</v>
+        <v>757211</v>
       </c>
       <c r="L19" s="3" t="n">
         <f aca="false">((G19*(D19/100))/I19)*100</f>
-        <v>0.616076392356941</v>
+        <v>0.614896921519474</v>
       </c>
       <c r="M19" s="3" t="n">
         <f aca="false">((G19*(E19/100))/I19)*100</f>
-        <v>0.351531894903401</v>
+        <v>0.35318534517429</v>
       </c>
       <c r="N19" s="3" t="n">
         <f aca="false">H19/I19</f>
@@ -1584,41 +1579,41 @@
         <v>0.99</v>
       </c>
       <c r="D21" s="2" t="n">
-        <v>0.447045599066689</v>
+        <v>0.44725714243048</v>
       </c>
       <c r="E21" s="2" t="n">
-        <v>0.535322127589263</v>
+        <v>0.535101757390073</v>
       </c>
       <c r="F21" s="2" t="n">
         <f aca="false">1-(D21+E21)</f>
-        <v>0.0176322733440484</v>
+        <v>0.0176411001794474</v>
       </c>
       <c r="G21" s="0" t="n">
-        <v>798876</v>
+        <v>803578</v>
       </c>
       <c r="H21" s="1" t="n">
         <f aca="false">(G21/C21)-G21</f>
-        <v>8069.45454545459</v>
+        <v>8116.94949494954</v>
       </c>
       <c r="I21" s="1" t="n">
         <f aca="false">G21+H21</f>
-        <v>806945.454545455</v>
+        <v>811694.94949495</v>
       </c>
       <c r="J21" s="1" t="n">
         <f aca="false">G21*D21</f>
-        <v>357134</v>
+        <v>359406</v>
       </c>
       <c r="K21" s="1" t="n">
         <f aca="false">G21*E21</f>
-        <v>427656</v>
+        <v>429996</v>
       </c>
       <c r="L21" s="3" t="n">
         <f aca="false">((G21*(D21/100))/I21)*100</f>
-        <v>0.442575143076022</v>
+        <v>0.442784571006175</v>
       </c>
       <c r="M21" s="3" t="n">
         <f aca="false">((G21*(E21/100))/I21)*100</f>
-        <v>0.52996890631337</v>
+        <v>0.529750739816172</v>
       </c>
       <c r="N21" s="3" t="n">
         <f aca="false">H21/I21</f>
@@ -1637,48 +1632,48 @@
         <v>10</v>
       </c>
       <c r="C22" s="2" t="n">
-        <v>0.75</v>
+        <v>0.76</v>
       </c>
       <c r="D22" s="2" t="n">
-        <v>0.360466689227237</v>
+        <v>0.356452407338998</v>
       </c>
       <c r="E22" s="2" t="n">
-        <v>0.629092080835155</v>
+        <v>0.633054954527064</v>
       </c>
       <c r="F22" s="2" t="n">
         <f aca="false">1-(D22+E22)</f>
-        <v>0.010441229937608</v>
+        <v>0.0104926381339385</v>
       </c>
       <c r="G22" s="0" t="n">
-        <v>2225121</v>
+        <v>2273880</v>
       </c>
       <c r="H22" s="1" t="n">
         <f aca="false">(G22/C22)-G22</f>
-        <v>741707</v>
+        <v>718067.368421053</v>
       </c>
       <c r="I22" s="1" t="n">
         <f aca="false">G22+H22</f>
-        <v>2966828</v>
+        <v>2991947.36842105</v>
       </c>
       <c r="J22" s="1" t="n">
         <f aca="false">G22*D22</f>
-        <v>802082</v>
+        <v>810530</v>
       </c>
       <c r="K22" s="1" t="n">
         <f aca="false">G22*E22</f>
-        <v>1399806</v>
+        <v>1439491</v>
       </c>
       <c r="L22" s="3" t="n">
         <f aca="false">((G22*(D22/100))/I22)*100</f>
-        <v>0.270350016920428</v>
+        <v>0.270903829577638</v>
       </c>
       <c r="M22" s="3" t="n">
         <f aca="false">((G22*(E22/100))/I22)*100</f>
-        <v>0.471819060626366</v>
+        <v>0.481121765440568</v>
       </c>
       <c r="N22" s="3" t="n">
         <f aca="false">H22/I22</f>
-        <v>0.25</v>
+        <v>0.24</v>
       </c>
       <c r="O22" s="0" t="str">
         <f aca="false">IF(SUM(MIN(L22,M22),N22)&lt;MAX(L22,M22),IF(MAX(L22,M22)=L22,"Trump","Biden"),"NONE")</f>
@@ -1696,25 +1691,25 @@
         <v>0.99</v>
       </c>
       <c r="D23" s="2" t="n">
-        <v>0.327196752347715</v>
+        <v>0.327203275971924</v>
       </c>
       <c r="E23" s="2" t="n">
-        <v>0.659743597703994</v>
+        <v>0.659756751622164</v>
       </c>
       <c r="F23" s="2" t="n">
         <f aca="false">1-(D23+E23)</f>
-        <v>0.0130596499482906</v>
+        <v>0.0130399724059123</v>
       </c>
       <c r="G23" s="0" t="n">
-        <v>3510967</v>
+        <v>3510897</v>
       </c>
       <c r="H23" s="1" t="n">
         <f aca="false">(G23/C23)-G23</f>
-        <v>35464.3131313133</v>
+        <v>35463.606060606</v>
       </c>
       <c r="I23" s="1" t="n">
         <f aca="false">G23+H23</f>
-        <v>3546431.31313131</v>
+        <v>3546360.60606061</v>
       </c>
       <c r="J23" s="1" t="n">
         <f aca="false">G23*D23</f>
@@ -1726,15 +1721,15 @@
       </c>
       <c r="L23" s="3" t="n">
         <f aca="false">((G23*(D23/100))/I23)*100</f>
-        <v>0.323924784824238</v>
+        <v>0.323931243212205</v>
       </c>
       <c r="M23" s="3" t="n">
         <f aca="false">((G23*(E23/100))/I23)*100</f>
-        <v>0.653146161726954</v>
+        <v>0.653159184105942</v>
       </c>
       <c r="N23" s="3" t="n">
         <f aca="false">H23/I23</f>
-        <v>0.01</v>
+        <v>0.00999999999999997</v>
       </c>
       <c r="O23" s="0" t="str">
         <f aca="false">IF(SUM(MIN(L23,M23),N23)&lt;MAX(L23,M23),IF(MAX(L23,M23)=L23,"Trump","Biden"),"NONE")</f>
@@ -1752,45 +1747,45 @@
         <v>0.99</v>
       </c>
       <c r="D24" s="2" t="n">
-        <v>0.481220272414274</v>
+        <v>0.481220323241249</v>
       </c>
       <c r="E24" s="2" t="n">
-        <v>0.507807167538254</v>
+        <v>0.507809534484999</v>
       </c>
       <c r="F24" s="2" t="n">
         <f aca="false">1-(D24+E24)</f>
-        <v>0.0109725600474713</v>
+        <v>0.0109701422737525</v>
       </c>
       <c r="G24" s="0" t="n">
-        <v>5495527</v>
+        <v>5495462</v>
       </c>
       <c r="H24" s="1" t="n">
         <f aca="false">(G24/C24)-G24</f>
-        <v>55510.3737373734</v>
+        <v>55509.7171717174</v>
       </c>
       <c r="I24" s="1" t="n">
         <f aca="false">G24+H24</f>
-        <v>5551037.37373737</v>
+        <v>5550971.71717172</v>
       </c>
       <c r="J24" s="1" t="n">
         <f aca="false">G24*D24</f>
-        <v>2644559</v>
+        <v>2644528</v>
       </c>
       <c r="K24" s="1" t="n">
         <f aca="false">G24*E24</f>
-        <v>2790668</v>
+        <v>2790648</v>
       </c>
       <c r="L24" s="3" t="n">
         <f aca="false">((G24*(D24/100))/I24)*100</f>
-        <v>0.476408069690132</v>
+        <v>0.476408120008836</v>
       </c>
       <c r="M24" s="3" t="n">
         <f aca="false">((G24*(E24/100))/I24)*100</f>
-        <v>0.502729095862872</v>
+        <v>0.502731439140149</v>
       </c>
       <c r="N24" s="3" t="n">
         <f aca="false">H24/I24</f>
-        <v>0.00999999999999994</v>
+        <v>0.01</v>
       </c>
       <c r="O24" s="0" t="str">
         <f aca="false">IF(SUM(MIN(L24,M24),N24)&lt;MAX(L24,M24),IF(MAX(L24,M24)=L24,"Trump","Biden"),"NONE")</f>
@@ -1808,41 +1803,41 @@
         <v>0.99</v>
       </c>
       <c r="D25" s="2" t="n">
-        <v>0.45856756216557</v>
+        <v>0.458572127610673</v>
       </c>
       <c r="E25" s="2" t="n">
-        <v>0.530624419029601</v>
+        <v>0.530619419380828</v>
       </c>
       <c r="F25" s="2" t="n">
         <f aca="false">1-(D25+E25)</f>
-        <v>0.0108080188048284</v>
+        <v>0.0108084530084989</v>
       </c>
       <c r="G25" s="0" t="n">
-        <v>3237041</v>
+        <v>3237096</v>
       </c>
       <c r="H25" s="1" t="n">
         <f aca="false">(G25/C25)-G25</f>
-        <v>32697.3838383839</v>
+        <v>32697.9393939395</v>
       </c>
       <c r="I25" s="1" t="n">
         <f aca="false">G25+H25</f>
-        <v>3269738.38383838</v>
+        <v>3269793.93939394</v>
       </c>
       <c r="J25" s="1" t="n">
         <f aca="false">G25*D25</f>
-        <v>1484402</v>
+        <v>1484442</v>
       </c>
       <c r="K25" s="1" t="n">
         <f aca="false">G25*E25</f>
-        <v>1717653</v>
+        <v>1717666</v>
       </c>
       <c r="L25" s="3" t="n">
         <f aca="false">((G25*(D25/100))/I25)*100</f>
-        <v>0.453981886543915</v>
+        <v>0.453986406334567</v>
       </c>
       <c r="M25" s="3" t="n">
         <f aca="false">((G25*(E25/100))/I25)*100</f>
-        <v>0.525318174839305</v>
+        <v>0.52531322518702</v>
       </c>
       <c r="N25" s="3" t="n">
         <f aca="false">H25/I25</f>
@@ -2085,48 +2080,48 @@
         <v>6</v>
       </c>
       <c r="C30" s="2" t="n">
-        <v>0.84</v>
+        <v>0.87</v>
       </c>
       <c r="D30" s="2" t="n">
-        <v>0.490450570897427</v>
+        <v>0.48698898478538</v>
       </c>
       <c r="E30" s="2" t="n">
-        <v>0.499913544263269</v>
+        <v>0.503145542203861</v>
       </c>
       <c r="F30" s="2" t="n">
         <f aca="false">1-(D30+E30)</f>
-        <v>0.009635884839304</v>
+        <v>0.00986547301075857</v>
       </c>
       <c r="G30" s="0" t="n">
-        <v>1208711</v>
+        <v>1246367</v>
       </c>
       <c r="H30" s="1" t="n">
         <f aca="false">(G30/C30)-G30</f>
-        <v>230230.666666667</v>
+        <v>186238.747126437</v>
       </c>
       <c r="I30" s="1" t="n">
         <f aca="false">G30+H30</f>
-        <v>1438941.66666667</v>
+        <v>1432605.74712644</v>
       </c>
       <c r="J30" s="1" t="n">
         <f aca="false">G30*D30</f>
-        <v>592813</v>
+        <v>606967</v>
       </c>
       <c r="K30" s="1" t="n">
         <f aca="false">G30*E30</f>
-        <v>604251</v>
+        <v>627104</v>
       </c>
       <c r="L30" s="3" t="n">
         <f aca="false">((G30*(D30/100))/I30)*100</f>
-        <v>0.411978479553839</v>
+        <v>0.423680416763281</v>
       </c>
       <c r="M30" s="3" t="n">
         <f aca="false">((G30*(E30/100))/I30)*100</f>
-        <v>0.419927377181146</v>
+        <v>0.437736621717359</v>
       </c>
       <c r="N30" s="3" t="n">
         <f aca="false">H30/I30</f>
-        <v>0.16</v>
+        <v>0.13</v>
       </c>
       <c r="O30" s="0" t="str">
         <f aca="false">IF(SUM(MIN(L30,M30),N30)&lt;MAX(L30,M30),IF(MAX(L30,M30)=L30,"Trump","Biden"),"NONE")</f>
@@ -2197,48 +2192,48 @@
         <v>14</v>
       </c>
       <c r="C32" s="2" t="n">
-        <v>0.71</v>
+        <v>0.74</v>
       </c>
       <c r="D32" s="2" t="n">
-        <v>0.393702744802261</v>
+        <v>0.399002776805958</v>
       </c>
       <c r="E32" s="2" t="n">
-        <v>0.600442069935577</v>
+        <v>0.594983577331435</v>
       </c>
       <c r="F32" s="2" t="n">
         <f aca="false">1-(D32+E32)</f>
-        <v>0.005855185262162</v>
+        <v>0.00601364586260744</v>
       </c>
       <c r="G32" s="0" t="n">
-        <v>3189993</v>
+        <v>3312799</v>
       </c>
       <c r="H32" s="1" t="n">
         <f aca="false">(G32/C32)-G32</f>
-        <v>1302954.88732394</v>
+        <v>1163956.40540541</v>
       </c>
       <c r="I32" s="1" t="n">
         <f aca="false">G32+H32</f>
-        <v>4492947.88732394</v>
+        <v>4476755.40540541</v>
       </c>
       <c r="J32" s="1" t="n">
         <f aca="false">G32*D32</f>
-        <v>1255909</v>
+        <v>1321816</v>
       </c>
       <c r="K32" s="1" t="n">
         <f aca="false">G32*E32</f>
-        <v>1915406</v>
+        <v>1971061</v>
       </c>
       <c r="L32" s="3" t="n">
         <f aca="false">((G32*(D32/100))/I32)*100</f>
-        <v>0.279528948809605</v>
+        <v>0.295262054836409</v>
       </c>
       <c r="M32" s="3" t="n">
         <f aca="false">((G32*(E32/100))/I32)*100</f>
-        <v>0.426313869654259</v>
+        <v>0.440287847225262</v>
       </c>
       <c r="N32" s="3" t="n">
         <f aca="false">H32/I32</f>
-        <v>0.29</v>
+        <v>0.26</v>
       </c>
       <c r="O32" s="0" t="str">
         <f aca="false">IF(SUM(MIN(L32,M32),N32)&lt;MAX(L32,M32),IF(MAX(L32,M32)=L32,"Trump","Biden"),"NONE")</f>
@@ -2312,41 +2307,41 @@
         <v>0.78</v>
       </c>
       <c r="D34" s="2" t="n">
-        <v>0.432181847096256</v>
+        <v>0.432227394389724</v>
       </c>
       <c r="E34" s="2" t="n">
-        <v>0.56056729189909</v>
+        <v>0.560521338705699</v>
       </c>
       <c r="F34" s="2" t="n">
         <f aca="false">1-(D34+E34)</f>
-        <v>0.00725086100465311</v>
+        <v>0.00725126690457745</v>
       </c>
       <c r="G34" s="0" t="n">
-        <v>6589976</v>
+        <v>6591262</v>
       </c>
       <c r="H34" s="1" t="n">
         <f aca="false">(G34/C34)-G34</f>
-        <v>1858711.17948718</v>
+        <v>1859073.8974359</v>
       </c>
       <c r="I34" s="1" t="n">
         <f aca="false">G34+H34</f>
-        <v>8448687.17948718</v>
+        <v>8450335.8974359</v>
       </c>
       <c r="J34" s="1" t="n">
         <f aca="false">G34*D34</f>
-        <v>2848068</v>
+        <v>2848924</v>
       </c>
       <c r="K34" s="1" t="n">
         <f aca="false">G34*E34</f>
-        <v>3694125</v>
+        <v>3694543</v>
       </c>
       <c r="L34" s="3" t="n">
         <f aca="false">((G34*(D34/100))/I34)*100</f>
-        <v>0.33710184073508</v>
+        <v>0.337137367623985</v>
       </c>
       <c r="M34" s="3" t="n">
         <f aca="false">((G34*(E34/100))/I34)*100</f>
-        <v>0.43724248768129</v>
+        <v>0.437206644190445</v>
       </c>
       <c r="N34" s="3" t="n">
         <f aca="false">H34/I34</f>
@@ -2645,48 +2640,48 @@
         <v>20</v>
       </c>
       <c r="C40" s="2" t="n">
-        <v>0.97</v>
+        <v>0.98</v>
       </c>
       <c r="D40" s="2" t="n">
-        <v>0.495618944308338</v>
+        <v>0.493268640317252</v>
       </c>
       <c r="E40" s="2" t="n">
-        <v>0.492897686780272</v>
+        <v>0.49526178756467</v>
       </c>
       <c r="F40" s="2" t="n">
         <f aca="false">1-(D40+E40)</f>
-        <v>0.0114833689113899</v>
+        <v>0.011469572118078</v>
       </c>
       <c r="G40" s="0" t="n">
-        <v>6630023</v>
+        <v>6684905</v>
       </c>
       <c r="H40" s="1" t="n">
         <f aca="false">(G40/C40)-G40</f>
-        <v>205052.257731959</v>
+        <v>136426.632653061</v>
       </c>
       <c r="I40" s="1" t="n">
         <f aca="false">G40+H40</f>
-        <v>6835075.25773196</v>
+        <v>6821331.63265306</v>
       </c>
       <c r="J40" s="1" t="n">
         <f aca="false">G40*D40</f>
-        <v>3285965</v>
+        <v>3297454</v>
       </c>
       <c r="K40" s="1" t="n">
         <f aca="false">G40*E40</f>
-        <v>3267923</v>
+        <v>3310778</v>
       </c>
       <c r="L40" s="3" t="n">
         <f aca="false">((G40*(D40/100))/I40)*100</f>
-        <v>0.480750375979088</v>
+        <v>0.483403267510907</v>
       </c>
       <c r="M40" s="3" t="n">
         <f aca="false">((G40*(E40/100))/I40)*100</f>
-        <v>0.478110756176864</v>
+        <v>0.485356551813377</v>
       </c>
       <c r="N40" s="3" t="n">
         <f aca="false">H40/I40</f>
-        <v>0.0300000000000001</v>
+        <v>0.02</v>
       </c>
       <c r="O40" s="0" t="str">
         <f aca="false">IF(SUM(MIN(L40,M40),N40)&lt;MAX(L40,M40),IF(MAX(L40,M40)=L40,"Trump","Biden"),"NONE")</f>
@@ -2928,41 +2923,41 @@
         <v>0.85</v>
       </c>
       <c r="D45" s="2" t="n">
-        <v>0.523386856291781</v>
+        <v>0.523384150030788</v>
       </c>
       <c r="E45" s="2" t="n">
-        <v>0.465435936016796</v>
+        <v>0.465438647333072</v>
       </c>
       <c r="F45" s="2" t="n">
         <f aca="false">1-(D45+E45)</f>
-        <v>0.0111772076914234</v>
+        <v>0.0111772026361394</v>
       </c>
       <c r="G45" s="0" t="n">
-        <v>11197251</v>
+        <v>11197435</v>
       </c>
       <c r="H45" s="1" t="n">
         <f aca="false">(G45/C45)-G45</f>
-        <v>1975985.47058824</v>
+        <v>1976017.94117647</v>
       </c>
       <c r="I45" s="1" t="n">
         <f aca="false">G45+H45</f>
-        <v>13173236.4705882</v>
+        <v>13173452.9411765</v>
       </c>
       <c r="J45" s="1" t="n">
         <f aca="false">G45*D45</f>
-        <v>5860494</v>
+        <v>5860560</v>
       </c>
       <c r="K45" s="1" t="n">
         <f aca="false">G45*E45</f>
-        <v>5211603</v>
+        <v>5211719</v>
       </c>
       <c r="L45" s="3" t="n">
         <f aca="false">((G45*(D45/100))/I45)*100</f>
-        <v>0.444878827848014</v>
+        <v>0.44487652752617</v>
       </c>
       <c r="M45" s="3" t="n">
         <f aca="false">((G45*(E45/100))/I45)*100</f>
-        <v>0.395620545614276</v>
+        <v>0.395622850233111</v>
       </c>
       <c r="N45" s="3" t="n">
         <f aca="false">H45/I45</f>
@@ -3264,45 +3259,45 @@
         <v>0.99</v>
       </c>
       <c r="D51" s="2" t="n">
-        <v>0.490968649064108</v>
+        <v>0.491010557140213</v>
       </c>
       <c r="E51" s="2" t="n">
-        <v>0.497315086208211</v>
+        <v>0.497274027275891</v>
       </c>
       <c r="F51" s="2" t="n">
         <f aca="false">1-(D51+E51)</f>
-        <v>0.0117162647276809</v>
+        <v>0.0117154155838967</v>
       </c>
       <c r="G51" s="0" t="n">
-        <v>3278690</v>
+        <v>3279013</v>
       </c>
       <c r="H51" s="1" t="n">
         <f aca="false">(G51/C51)-G51</f>
-        <v>33118.0808080807</v>
+        <v>33121.3434343436</v>
       </c>
       <c r="I51" s="1" t="n">
         <f aca="false">G51+H51</f>
-        <v>3311808.08080808</v>
+        <v>3312134.34343434</v>
       </c>
       <c r="J51" s="1" t="n">
         <f aca="false">G51*D51</f>
-        <v>1609734</v>
+        <v>1610030</v>
       </c>
       <c r="K51" s="1" t="n">
         <f aca="false">G51*E51</f>
-        <v>1630542</v>
+        <v>1630568</v>
       </c>
       <c r="L51" s="3" t="n">
         <f aca="false">((G51*(D51/100))/I51)*100</f>
-        <v>0.486058962573467</v>
+        <v>0.486100451568811</v>
       </c>
       <c r="M51" s="3" t="n">
         <f aca="false">((G51*(E51/100))/I51)*100</f>
-        <v>0.492341935346129</v>
+        <v>0.492301287003132</v>
       </c>
       <c r="N51" s="3" t="n">
         <f aca="false">H51/I51</f>
-        <v>0.00999999999999998</v>
+        <v>0.01</v>
       </c>
       <c r="O51" s="0" t="str">
         <f aca="false">IF(SUM(MIN(L51,M51),N51)&lt;MAX(L51,M51),IF(MAX(L51,M51)=L51,"Trump","Biden"),"NONE")</f>

</xml_diff>

<commit_message>
Correct math on %margin uncounted, updated README explaining congressional split not taken into account
</commit_message>
<xml_diff>
--- a/ElectionTracker2020.xlsx
+++ b/ElectionTracker2020.xlsx
@@ -402,11 +402,11 @@
   <dimension ref="A1:Q52"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
-      <selection pane="bottomRight" activeCell="G1" activeCellId="0" sqref="G:G G1"/>
+      <selection pane="topRight" activeCell="L1" activeCellId="0" sqref="L1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="N5" activeCellId="0" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -529,8 +529,8 @@
         <v>0.36077686085386</v>
       </c>
       <c r="N2" s="3" t="n">
-        <f aca="false">H2/I2</f>
-        <v>0.00999999999999998</v>
+        <f aca="false">1-L2-M2</f>
+        <v>0.020765380624832</v>
       </c>
       <c r="O2" s="0" t="str">
         <f aca="false">IF(SUM(MIN(L2,M2),N2)&lt;MAX(L2,M2),IF(MAX(L2,M2)=L2,"Trump","Biden"),"NONE")</f>
@@ -538,7 +538,7 @@
       </c>
       <c r="P2" s="1" t="n">
         <f aca="false">SUMIF(O2:O52,"Trump",B2:B52)</f>
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="Q2" s="0" t="n">
         <f aca="false">SUMIF(O2:O52,"Biden",B2:B52)</f>
@@ -593,8 +593,8 @@
         <v>0.170379994887961</v>
       </c>
       <c r="N3" s="3" t="n">
-        <f aca="false">H3/I3</f>
-        <v>0.5</v>
+        <f aca="false">1-L3-M3</f>
+        <v>0.513839780182329</v>
       </c>
       <c r="O3" s="0" t="str">
         <f aca="false">IF(SUM(MIN(L3,M3),N3)&lt;MAX(L3,M3),IF(MAX(L3,M3)=L3,"Trump","Biden"),"NONE")</f>
@@ -649,8 +649,8 @@
         <v>0.449865859808371</v>
       </c>
       <c r="N4" s="3" t="n">
-        <f aca="false">H4/I4</f>
-        <v>0.1</v>
+        <f aca="false">1-L4-M4</f>
+        <v>0.112883797997262</v>
       </c>
       <c r="O4" s="0" t="str">
         <f aca="false">IF(SUM(MIN(L4,M4),N4)&lt;MAX(L4,M4),IF(MAX(L4,M4)=L4,"Trump","Biden"),"NONE")</f>
@@ -711,8 +711,8 @@
         <v>0.348614014228764</v>
       </c>
       <c r="N5" s="3" t="n">
-        <f aca="false">H5/I5</f>
-        <v>0.0100000000000001</v>
+        <f aca="false">1-L5-M5</f>
+        <v>0.0208772691154249</v>
       </c>
       <c r="O5" s="0" t="str">
         <f aca="false">IF(SUM(MIN(L5,M5),N5)&lt;MAX(L5,M5),IF(MAX(L5,M5)=L5,"Trump","Biden"),"NONE")</f>
@@ -775,8 +775,8 @@
         <v>0.433685436955448</v>
       </c>
       <c r="N6" s="3" t="n">
-        <f aca="false">H6/I6</f>
-        <v>0.34</v>
+        <f aca="false">1-L6-M6</f>
+        <v>0.346146898305476</v>
       </c>
       <c r="O6" s="0" t="str">
         <f aca="false">IF(SUM(MIN(L6,M6),N6)&lt;MAX(L6,M6),IF(MAX(L6,M6)=L6,"Trump","Biden"),"NONE")</f>
@@ -831,8 +831,8 @@
         <v>0.518535777151487</v>
       </c>
       <c r="N7" s="3" t="n">
-        <f aca="false">H7/I7</f>
-        <v>0.07</v>
+        <f aca="false">1-L7-M7</f>
+        <v>0.0848841029981819</v>
       </c>
       <c r="O7" s="0" t="str">
         <f aca="false">IF(SUM(MIN(L7,M7),N7)&lt;MAX(L7,M7),IF(MAX(L7,M7)=L7,"Trump","Biden"),"NONE")</f>
@@ -888,8 +888,8 @@
         <v>0.577325852433523</v>
       </c>
       <c r="N8" s="3" t="n">
-        <f aca="false">H8/I8</f>
-        <v>0.00999999999999996</v>
+        <f aca="false">1-L8-M8</f>
+        <v>0.0210861161743739</v>
       </c>
       <c r="O8" s="0" t="str">
         <f aca="false">IF(SUM(MIN(L8,M8),N8)&lt;MAX(L8,M8),IF(MAX(L8,M8)=L8,"Trump","Biden"),"NONE")</f>
@@ -944,8 +944,8 @@
         <v>0.584653554814088</v>
       </c>
       <c r="N9" s="3" t="n">
-        <f aca="false">H9/I9</f>
-        <v>0.01</v>
+        <f aca="false">1-L9-M9</f>
+        <v>0.0198503425568108</v>
       </c>
       <c r="O9" s="0" t="str">
         <f aca="false">IF(SUM(MIN(L9,M9),N9)&lt;MAX(L9,M9),IF(MAX(L9,M9)=L9,"Trump","Biden"),"NONE")</f>
@@ -1000,8 +1000,8 @@
         <v>0.781675092556235</v>
       </c>
       <c r="N10" s="3" t="n">
-        <f aca="false">H10/I10</f>
-        <v>0.17</v>
+        <f aca="false">1-L10-M10</f>
+        <v>0.174457985078813</v>
       </c>
       <c r="O10" s="0" t="str">
         <f aca="false">IF(SUM(MIN(L10,M10),N10)&lt;MAX(L10,M10),IF(MAX(L10,M10)=L10,"Trump","Biden"),"NONE")</f>
@@ -1056,8 +1056,8 @@
         <v>0.475027783251053</v>
       </c>
       <c r="N11" s="3" t="n">
-        <f aca="false">H11/I11</f>
-        <v>0.01</v>
+        <f aca="false">1-L11-M11</f>
+        <v>0.0162963658766689</v>
       </c>
       <c r="O11" s="0" t="str">
         <f aca="false">IF(SUM(MIN(L11,M11),N11)&lt;MAX(L11,M11),IF(MAX(L11,M11)=L11,"Trump","Biden"),"NONE")</f>
@@ -1112,8 +1112,8 @@
         <v>0.489028930559963</v>
       </c>
       <c r="N12" s="3" t="n">
-        <f aca="false">H12/I12</f>
-        <v>0.00999999999999995</v>
+        <f aca="false">1-L12-M12</f>
+        <v>0.022252897148555</v>
       </c>
       <c r="O12" s="0" t="str">
         <f aca="false">IF(SUM(MIN(L12,M12),N12)&lt;MAX(L12,M12),IF(MAX(L12,M12)=L12,"Trump","Biden"),"NONE")</f>
@@ -1168,8 +1168,8 @@
         <v>0.618334193182598</v>
       </c>
       <c r="N13" s="3" t="n">
-        <f aca="false">H13/I13</f>
-        <v>0.0400000000000001</v>
+        <f aca="false">1-L13-M13</f>
+        <v>0.0493391955684609</v>
       </c>
       <c r="O13" s="0" t="str">
         <f aca="false">IF(SUM(MIN(L13,M13),N13)&lt;MAX(L13,M13),IF(MAX(L13,M13)=L13,"Trump","Biden"),"NONE")</f>
@@ -1224,8 +1224,8 @@
         <v>0.331370941123918</v>
       </c>
       <c r="N14" s="3" t="n">
-        <f aca="false">H14/I14</f>
-        <v>0.01</v>
+        <f aca="false">1-L14-M14</f>
+        <v>0.0289372308029639</v>
       </c>
       <c r="O14" s="0" t="str">
         <f aca="false">IF(SUM(MIN(L14,M14),N14)&lt;MAX(L14,M14),IF(MAX(L14,M14)=L14,"Trump","Biden"),"NONE")</f>
@@ -1280,8 +1280,8 @@
         <v>0.509826999967664</v>
       </c>
       <c r="N15" s="3" t="n">
-        <f aca="false">H15/I15</f>
-        <v>0.09</v>
+        <f aca="false">1-L15-M15</f>
+        <v>0.100057287861175</v>
       </c>
       <c r="O15" s="0" t="str">
         <f aca="false">IF(SUM(MIN(L15,M15),N15)&lt;MAX(L15,M15),IF(MAX(L15,M15)=L15,"Trump","Biden"),"NONE")</f>
@@ -1336,8 +1336,8 @@
         <v>0.405743985172289</v>
       </c>
       <c r="N16" s="3" t="n">
-        <f aca="false">H16/I16</f>
-        <v>0.00999999999999994</v>
+        <f aca="false">1-L16-M16</f>
+        <v>0.0292205893247879</v>
       </c>
       <c r="O16" s="0" t="str">
         <f aca="false">IF(SUM(MIN(L16,M16),N16)&lt;MAX(L16,M16),IF(MAX(L16,M16)=L16,"Trump","Biden"),"NONE")</f>
@@ -1392,8 +1392,8 @@
         <v>0.448283344011322</v>
       </c>
       <c r="N17" s="3" t="n">
-        <f aca="false">H17/I17</f>
-        <v>0.01</v>
+        <f aca="false">1-L17-M17</f>
+        <v>0.0215701484081029</v>
       </c>
       <c r="O17" s="0" t="str">
         <f aca="false">IF(SUM(MIN(L17,M17),N17)&lt;MAX(L17,M17),IF(MAX(L17,M17)=L17,"Trump","Biden"),"NONE")</f>
@@ -1448,8 +1448,8 @@
         <v>0.408503807893272</v>
       </c>
       <c r="N18" s="3" t="n">
-        <f aca="false">H18/I18</f>
-        <v>0.01</v>
+        <f aca="false">1-L18-M18</f>
+        <v>0.0318388987351209</v>
       </c>
       <c r="O18" s="0" t="str">
         <f aca="false">IF(SUM(MIN(L18,M18),N18)&lt;MAX(L18,M18),IF(MAX(L18,M18)=L18,"Trump","Biden"),"NONE")</f>
@@ -1504,8 +1504,8 @@
         <v>0.35318534517429</v>
       </c>
       <c r="N19" s="3" t="n">
-        <f aca="false">H19/I19</f>
-        <v>0.02</v>
+        <f aca="false">1-L19-M19</f>
+        <v>0.0319177333062359</v>
       </c>
       <c r="O19" s="0" t="str">
         <f aca="false">IF(SUM(MIN(L19,M19),N19)&lt;MAX(L19,M19),IF(MAX(L19,M19)=L19,"Trump","Biden"),"NONE")</f>
@@ -1560,8 +1560,8 @@
         <v>0.381118682580037</v>
       </c>
       <c r="N20" s="3" t="n">
-        <f aca="false">H20/I20</f>
-        <v>0.05</v>
+        <f aca="false">1-L20-M20</f>
+        <v>0.0596375791596989</v>
       </c>
       <c r="O20" s="0" t="str">
         <f aca="false">IF(SUM(MIN(L20,M20),N20)&lt;MAX(L20,M20),IF(MAX(L20,M20)=L20,"Trump","Biden"),"NONE")</f>
@@ -1616,8 +1616,8 @@
         <v>0.529750739816172</v>
       </c>
       <c r="N21" s="3" t="n">
-        <f aca="false">H21/I21</f>
-        <v>0.0100000000000001</v>
+        <f aca="false">1-L21-M21</f>
+        <v>0.0274646891776529</v>
       </c>
       <c r="O21" s="0" t="str">
         <f aca="false">IF(SUM(MIN(L21,M21),N21)&lt;MAX(L21,M21),IF(MAX(L21,M21)=L21,"Trump","Biden"),"NONE")</f>
@@ -1672,8 +1672,8 @@
         <v>0.481121765440568</v>
       </c>
       <c r="N22" s="3" t="n">
-        <f aca="false">H22/I22</f>
-        <v>0.24</v>
+        <f aca="false">1-L22-M22</f>
+        <v>0.247974404981794</v>
       </c>
       <c r="O22" s="0" t="str">
         <f aca="false">IF(SUM(MIN(L22,M22),N22)&lt;MAX(L22,M22),IF(MAX(L22,M22)=L22,"Trump","Biden"),"NONE")</f>
@@ -1728,8 +1728,8 @@
         <v>0.653159184105942</v>
       </c>
       <c r="N23" s="3" t="n">
-        <f aca="false">H23/I23</f>
-        <v>0.00999999999999997</v>
+        <f aca="false">1-L23-M23</f>
+        <v>0.0229095726818529</v>
       </c>
       <c r="O23" s="0" t="str">
         <f aca="false">IF(SUM(MIN(L23,M23),N23)&lt;MAX(L23,M23),IF(MAX(L23,M23)=L23,"Trump","Biden"),"NONE")</f>
@@ -1784,8 +1784,8 @@
         <v>0.502731439140149</v>
       </c>
       <c r="N24" s="3" t="n">
-        <f aca="false">H24/I24</f>
-        <v>0.01</v>
+        <f aca="false">1-L24-M24</f>
+        <v>0.0208604408510149</v>
       </c>
       <c r="O24" s="0" t="str">
         <f aca="false">IF(SUM(MIN(L24,M24),N24)&lt;MAX(L24,M24),IF(MAX(L24,M24)=L24,"Trump","Biden"),"NONE")</f>
@@ -1840,8 +1840,8 @@
         <v>0.52531322518702</v>
       </c>
       <c r="N25" s="3" t="n">
-        <f aca="false">H25/I25</f>
-        <v>0.01</v>
+        <f aca="false">1-L25-M25</f>
+        <v>0.0207003684784129</v>
       </c>
       <c r="O25" s="0" t="str">
         <f aca="false">IF(SUM(MIN(L25,M25),N25)&lt;MAX(L25,M25),IF(MAX(L25,M25)=L25,"Trump","Biden"),"NONE")</f>
@@ -1896,8 +1896,8 @@
         <v>0.328800625171695</v>
       </c>
       <c r="N26" s="3" t="n">
-        <f aca="false">H26/I26</f>
-        <v>0.16</v>
+        <f aca="false">1-L26-M26</f>
+        <v>0.165458303661682</v>
       </c>
       <c r="O26" s="0" t="str">
         <f aca="false">IF(SUM(MIN(L26,M26),N26)&lt;MAX(L26,M26),IF(MAX(L26,M26)=L26,"Trump","Biden"),"NONE")</f>
@@ -1952,8 +1952,8 @@
         <v>0.410739002901225</v>
       </c>
       <c r="N27" s="3" t="n">
-        <f aca="false">H27/I27</f>
-        <v>0.01</v>
+        <f aca="false">1-L27-M27</f>
+        <v>0.0235272601999379</v>
       </c>
       <c r="O27" s="0" t="str">
         <f aca="false">IF(SUM(MIN(L27,M27),N27)&lt;MAX(L27,M27),IF(MAX(L27,M27)=L27,"Trump","Biden"),"NONE")</f>
@@ -2008,8 +2008,8 @@
         <v>0.401681111407072</v>
       </c>
       <c r="N28" s="3" t="n">
-        <f aca="false">H28/I28</f>
-        <v>0.01</v>
+        <f aca="false">1-L28-M28</f>
+        <v>0.035041719384697</v>
       </c>
       <c r="O28" s="0" t="str">
         <f aca="false">IF(SUM(MIN(L28,M28),N28)&lt;MAX(L28,M28),IF(MAX(L28,M28)=L28,"Trump","Biden"),"NONE")</f>
@@ -2064,8 +2064,8 @@
         <v>0.387218263790378</v>
       </c>
       <c r="N29" s="3" t="n">
-        <f aca="false">H29/I29</f>
-        <v>0.00999999999999997</v>
+        <f aca="false">1-L29-M29</f>
+        <v>0.0307981170949159</v>
       </c>
       <c r="O29" s="0" t="str">
         <f aca="false">IF(SUM(MIN(L29,M29),N29)&lt;MAX(L29,M29),IF(MAX(L29,M29)=L29,"Trump","Biden"),"NONE")</f>
@@ -2120,8 +2120,8 @@
         <v>0.437736621717359</v>
       </c>
       <c r="N30" s="3" t="n">
-        <f aca="false">H30/I30</f>
-        <v>0.13</v>
+        <f aca="false">1-L30-M30</f>
+        <v>0.13858296151936</v>
       </c>
       <c r="O30" s="0" t="str">
         <f aca="false">IF(SUM(MIN(L30,M30),N30)&lt;MAX(L30,M30),IF(MAX(L30,M30)=L30,"Trump","Biden"),"NONE")</f>
@@ -2176,8 +2176,8 @@
         <v>0.522696937334378</v>
       </c>
       <c r="N31" s="3" t="n">
-        <f aca="false">H31/I31</f>
-        <v>0.0100000000000001</v>
+        <f aca="false">1-L31-M31</f>
+        <v>0.0261322555531709</v>
       </c>
       <c r="O31" s="0" t="str">
         <f aca="false">IF(SUM(MIN(L31,M31),N31)&lt;MAX(L31,M31),IF(MAX(L31,M31)=L31,"Trump","Biden"),"NONE")</f>
@@ -2232,8 +2232,8 @@
         <v>0.440287847225262</v>
       </c>
       <c r="N32" s="3" t="n">
-        <f aca="false">H32/I32</f>
-        <v>0.26</v>
+        <f aca="false">1-L32-M32</f>
+        <v>0.264450097938329</v>
       </c>
       <c r="O32" s="0" t="str">
         <f aca="false">IF(SUM(MIN(L32,M32),N32)&lt;MAX(L32,M32),IF(MAX(L32,M32)=L32,"Trump","Biden"),"NONE")</f>
@@ -2288,8 +2288,8 @@
         <v>0.540879248972087</v>
       </c>
       <c r="N33" s="3" t="n">
-        <f aca="false">H33/I33</f>
-        <v>0.00999999999999997</v>
+        <f aca="false">1-L33-M33</f>
+        <v>0.0235495789928599</v>
       </c>
       <c r="O33" s="0" t="str">
         <f aca="false">IF(SUM(MIN(L33,M33),N33)&lt;MAX(L33,M33),IF(MAX(L33,M33)=L33,"Trump","Biden"),"NONE")</f>
@@ -2344,8 +2344,8 @@
         <v>0.437206644190445</v>
       </c>
       <c r="N34" s="3" t="n">
-        <f aca="false">H34/I34</f>
-        <v>0.22</v>
+        <f aca="false">1-L34-M34</f>
+        <v>0.22565598818557</v>
       </c>
       <c r="O34" s="0" t="str">
         <f aca="false">IF(SUM(MIN(L34,M34),N34)&lt;MAX(L34,M34),IF(MAX(L34,M34)=L34,"Trump","Biden"),"NONE")</f>
@@ -2400,8 +2400,8 @@
         <v>0.459283545937002</v>
       </c>
       <c r="N35" s="3" t="n">
-        <f aca="false">H35/I35</f>
-        <v>0.06</v>
+        <f aca="false">1-L35-M35</f>
+        <v>0.0681664575774629</v>
       </c>
       <c r="O35" s="0" t="str">
         <f aca="false">IF(SUM(MIN(L35,M35),N35)&lt;MAX(L35,M35),IF(MAX(L35,M35)=L35,"Trump","Biden"),"NONE")</f>
@@ -2456,8 +2456,8 @@
         <v>0.315985635901325</v>
       </c>
       <c r="N36" s="3" t="n">
-        <f aca="false">H36/I36</f>
-        <v>0.00999999999999997</v>
+        <f aca="false">1-L36-M36</f>
+        <v>0.0357994211981979</v>
       </c>
       <c r="O36" s="0" t="str">
         <f aca="false">IF(SUM(MIN(L36,M36),N36)&lt;MAX(L36,M36),IF(MAX(L36,M36)=L36,"Trump","Biden"),"NONE")</f>
@@ -2512,8 +2512,8 @@
         <v>0.435223207616357</v>
       </c>
       <c r="N37" s="3" t="n">
-        <f aca="false">H37/I37</f>
-        <v>0.04</v>
+        <f aca="false">1-L37-M37</f>
+        <v>0.0508765225349269</v>
       </c>
       <c r="O37" s="0" t="str">
         <f aca="false">IF(SUM(MIN(L37,M37),N37)&lt;MAX(L37,M37),IF(MAX(L37,M37)=L37,"Trump","Biden"),"NONE")</f>
@@ -2568,8 +2568,8 @@
         <v>0.322111207005227</v>
       </c>
       <c r="N38" s="3" t="n">
-        <f aca="false">H38/I38</f>
-        <v>0.01</v>
+        <f aca="false">1-L38-M38</f>
+        <v>0.0257993464115669</v>
       </c>
       <c r="O38" s="0" t="str">
         <f aca="false">IF(SUM(MIN(L38,M38),N38)&lt;MAX(L38,M38),IF(MAX(L38,M38)=L38,"Trump","Biden"),"NONE")</f>
@@ -2624,8 +2624,8 @@
         <v>0.522768264636137</v>
       </c>
       <c r="N39" s="3" t="n">
-        <f aca="false">H39/I39</f>
-        <v>0.0899999999999999</v>
+        <f aca="false">1-L39-M39</f>
+        <v>0.105724700140744</v>
       </c>
       <c r="O39" s="0" t="str">
         <f aca="false">IF(SUM(MIN(L39,M39),N39)&lt;MAX(L39,M39),IF(MAX(L39,M39)=L39,"Trump","Biden"),"NONE")</f>
@@ -2680,8 +2680,8 @@
         <v>0.485356551813377</v>
       </c>
       <c r="N40" s="3" t="n">
-        <f aca="false">H40/I40</f>
-        <v>0.02</v>
+        <f aca="false">1-L40-M40</f>
+        <v>0.0312401806757159</v>
       </c>
       <c r="O40" s="0" t="str">
         <f aca="false">IF(SUM(MIN(L40,M40),N40)&lt;MAX(L40,M40),IF(MAX(L40,M40)=L40,"Trump","Biden"),"NONE")</f>
@@ -2736,8 +2736,8 @@
         <v>0.560784117631702</v>
       </c>
       <c r="N41" s="3" t="n">
-        <f aca="false">H41/I41</f>
-        <v>0.0599999999999999</v>
+        <f aca="false">1-L41-M41</f>
+        <v>0.069232731077333</v>
       </c>
       <c r="O41" s="0" t="str">
         <f aca="false">IF(SUM(MIN(L41,M41),N41)&lt;MAX(L41,M41),IF(MAX(L41,M41)=L41,"Trump","Biden"),"NONE")</f>
@@ -2792,8 +2792,8 @@
         <v>0.409968193044831</v>
       </c>
       <c r="N42" s="3" t="n">
-        <f aca="false">H42/I42</f>
-        <v>0.06</v>
+        <f aca="false">1-L42-M42</f>
+        <v>0.0707505021359079</v>
       </c>
       <c r="O42" s="0" t="str">
         <f aca="false">IF(SUM(MIN(L42,M42),N42)&lt;MAX(L42,M42),IF(MAX(L42,M42)=L42,"Trump","Biden"),"NONE")</f>
@@ -2848,8 +2848,8 @@
         <v>0.334675618177214</v>
       </c>
       <c r="N43" s="3" t="n">
-        <f aca="false">H43/I43</f>
-        <v>0.06</v>
+        <f aca="false">1-L43-M43</f>
+        <v>0.0846782449422949</v>
       </c>
       <c r="O43" s="0" t="str">
         <f aca="false">IF(SUM(MIN(L43,M43),N43)&lt;MAX(L43,M43),IF(MAX(L43,M43)=L43,"Trump","Biden"),"NONE")</f>
@@ -2904,8 +2904,8 @@
         <v>0.366210151214449</v>
       </c>
       <c r="N44" s="3" t="n">
-        <f aca="false">H44/I44</f>
-        <v>0.03</v>
+        <f aca="false">1-L44-M44</f>
+        <v>0.0395808086479809</v>
       </c>
       <c r="O44" s="0" t="str">
         <f aca="false">IF(SUM(MIN(L44,M44),N44)&lt;MAX(L44,M44),IF(MAX(L44,M44)=L44,"Trump","Biden"),"NONE")</f>
@@ -2960,8 +2960,8 @@
         <v>0.395622850233111</v>
       </c>
       <c r="N45" s="3" t="n">
-        <f aca="false">H45/I45</f>
-        <v>0.15</v>
+        <f aca="false">1-L45-M45</f>
+        <v>0.159500622240719</v>
       </c>
       <c r="O45" s="0" t="str">
         <f aca="false">IF(SUM(MIN(L45,M45),N45)&lt;MAX(L45,M45),IF(MAX(L45,M45)=L45,"Trump","Biden"),"NONE")</f>
@@ -3016,12 +3016,12 @@
         <v>0.316958977843852</v>
       </c>
       <c r="N46" s="3" t="n">
-        <f aca="false">H46/I46</f>
-        <v>0.17</v>
+        <f aca="false">1-L46-M46</f>
+        <v>0.189097698291402</v>
       </c>
       <c r="O46" s="0" t="str">
         <f aca="false">IF(SUM(MIN(L46,M46),N46)&lt;MAX(L46,M46),IF(MAX(L46,M46)=L46,"Trump","Biden"),"NONE")</f>
-        <v>Trump</v>
+        <v>NONE</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3072,8 +3072,8 @@
         <v>0.622115711317697</v>
       </c>
       <c r="N47" s="3" t="n">
-        <f aca="false">H47/I47</f>
-        <v>0.08</v>
+        <f aca="false">1-L47-M47</f>
+        <v>0.0891547514941539</v>
       </c>
       <c r="O47" s="0" t="str">
         <f aca="false">IF(SUM(MIN(L47,M47),N47)&lt;MAX(L47,M47),IF(MAX(L47,M47)=L47,"Trump","Biden"),"NONE")</f>
@@ -3128,8 +3128,8 @@
         <v>0.534418774965482</v>
       </c>
       <c r="N48" s="3" t="n">
-        <f aca="false">H48/I48</f>
-        <v>0.0100000000000001</v>
+        <f aca="false">1-L48-M48</f>
+        <v>0.0245010180009899</v>
       </c>
       <c r="O48" s="0" t="str">
         <f aca="false">IF(SUM(MIN(L48,M48),N48)&lt;MAX(L48,M48),IF(MAX(L48,M48)=L48,"Trump","Biden"),"NONE")</f>
@@ -3184,8 +3184,8 @@
         <v>0.508780779203218</v>
       </c>
       <c r="N49" s="3" t="n">
-        <f aca="false">H49/I49</f>
-        <v>0.15</v>
+        <f aca="false">1-L49-M49</f>
+        <v>0.165974706964385</v>
       </c>
       <c r="O49" s="0" t="str">
         <f aca="false">IF(SUM(MIN(L49,M49),N49)&lt;MAX(L49,M49),IF(MAX(L49,M49)=L49,"Trump","Biden"),"NONE")</f>
@@ -3240,8 +3240,8 @@
         <v>0.294128069677756</v>
       </c>
       <c r="N50" s="3" t="n">
-        <f aca="false">H50/I50</f>
-        <v>0.00999999999999996</v>
+        <f aca="false">1-L50-M50</f>
+        <v>0.023235016752409</v>
       </c>
       <c r="O50" s="0" t="str">
         <f aca="false">IF(SUM(MIN(L50,M50),N50)&lt;MAX(L50,M50),IF(MAX(L50,M50)=L50,"Trump","Biden"),"NONE")</f>
@@ -3296,8 +3296,8 @@
         <v>0.492301287003132</v>
       </c>
       <c r="N51" s="3" t="n">
-        <f aca="false">H51/I51</f>
-        <v>0.01</v>
+        <f aca="false">1-L51-M51</f>
+        <v>0.021598261428057</v>
       </c>
       <c r="O51" s="0" t="str">
         <f aca="false">IF(SUM(MIN(L51,M51),N51)&lt;MAX(L51,M51),IF(MAX(L51,M51)=L51,"Trump","Biden"),"NONE")</f>
@@ -3352,8 +3352,8 @@
         <v>0.261280000293401</v>
       </c>
       <c r="N52" s="3" t="n">
-        <f aca="false">H52/I52</f>
-        <v>0.03</v>
+        <f aca="false">1-L52-M52</f>
+        <v>0.0505089414077399</v>
       </c>
       <c r="O52" s="0" t="str">
         <f aca="false">IF(SUM(MIN(L52,M52),N52)&lt;MAX(L52,M52),IF(MAX(L52,M52)=L52,"Trump","Biden"),"NONE")</f>

</xml_diff>